<commit_message>
Sensor Index and NOAA update
</commit_message>
<xml_diff>
--- a/arcpy/qaqc/Historic_PurpleAir/PA IDs and indexes.xlsx
+++ b/arcpy/qaqc/Historic_PurpleAir/PA IDs and indexes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tande\Documents\GitHub\QualityAirQualityCities\arcpy\qaqc\Historic_PurpleAir\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B4FF4C3-CCE2-4614-BDB1-CA02CA3414AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7CC4166-4456-49AF-B2BD-9F0C78196B80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{AFF7FDF3-5C8E-44D7-B59C-1262BA8F9470}"/>
+    <workbookView xWindow="19090" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{AFF7FDF3-5C8E-44D7-B59C-1262BA8F9470}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -835,8 +835,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B394A7EB-A1AA-4267-B057-34339BEFEB84}">
   <dimension ref="A1:D126"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>